<commit_message>
Actualizacion de tabla de errores y mejor de cogido pasabajas
</commit_message>
<xml_diff>
--- a/Tabla errores.xlsx
+++ b/Tabla errores.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t xml:space="preserve">Señal </t>
   </si>
@@ -103,7 +103,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -325,18 +325,18 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -617,16 +617,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E22"/>
+  <dimension ref="B2:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
@@ -639,8 +642,20 @@
       <c r="E3" s="13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
@@ -653,8 +668,20 @@
       <c r="E4" s="12">
         <v>5.3999999999999999E-2</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="10">
+        <v>9.6450999999999993</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0.2666</v>
+      </c>
+      <c r="K4" s="12">
+        <v>0.1084</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
@@ -667,8 +694,20 @@
       <c r="E5" s="2">
         <v>2.8799999999999999E-2</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="5">
+        <v>10.252800000000001</v>
+      </c>
+      <c r="J5" s="1">
+        <v>-1.8517999999999999</v>
+      </c>
+      <c r="K5" s="2">
+        <v>9.4299999999999995E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>3</v>
       </c>
@@ -681,8 +720,20 @@
       <c r="E6" s="2">
         <v>4.1399999999999999E-2</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="5">
+        <v>8.2516999999999996</v>
+      </c>
+      <c r="J6" s="1">
+        <v>-2.3271000000000002</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.14960000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -695,8 +746,20 @@
       <c r="E7" s="2">
         <v>1.9199999999999998E-2</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="5">
+        <v>12.3062</v>
+      </c>
+      <c r="J7" s="1">
+        <v>-1.5971</v>
+      </c>
+      <c r="K7" s="2">
+        <v>5.8799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
         <v>5</v>
       </c>
@@ -709,8 +772,20 @@
       <c r="E8" s="2">
         <v>2.0400000000000001E-2</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="5">
+        <v>10.3828</v>
+      </c>
+      <c r="J8" s="1">
+        <v>-3.2709000000000001</v>
+      </c>
+      <c r="K8" s="2">
+        <v>9.1600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
         <v>6</v>
       </c>
@@ -723,8 +798,20 @@
       <c r="E9" s="2">
         <v>2.01E-2</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="5">
+        <v>11.0802</v>
+      </c>
+      <c r="J9" s="1">
+        <v>-2.6181000000000001</v>
+      </c>
+      <c r="K9" s="2">
+        <v>7.8E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
@@ -737,8 +824,20 @@
       <c r="E10" s="2">
         <v>2.3E-2</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="5">
+        <v>11.3095</v>
+      </c>
+      <c r="J10" s="1">
+        <v>-1.782</v>
+      </c>
+      <c r="K10" s="2">
+        <v>7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
@@ -751,8 +850,20 @@
       <c r="E11" s="2">
         <v>5.6500000000000002E-2</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="5">
+        <v>9.1279000000000003</v>
+      </c>
+      <c r="J11" s="1">
+        <v>-5.79E-2</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.1222</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
@@ -765,8 +876,20 @@
       <c r="E12" s="2">
         <v>3.3700000000000001E-2</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="5">
+        <v>9.8223000000000003</v>
+      </c>
+      <c r="J12" s="1">
+        <v>-1.6224000000000001</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.1042</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
         <v>10</v>
       </c>
@@ -779,8 +902,20 @@
       <c r="E13" s="2">
         <v>1.9E-2</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="5">
+        <v>12.023899999999999</v>
+      </c>
+      <c r="J13" s="1">
+        <v>-1.9446000000000001</v>
+      </c>
+      <c r="K13" s="2">
+        <v>6.2700000000000006E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
         <v>11</v>
       </c>
@@ -793,8 +928,20 @@
       <c r="E14" s="2">
         <v>5.3100000000000001E-2</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="5">
+        <v>10.028</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.56120000000000003</v>
+      </c>
+      <c r="K14" s="2">
+        <v>9.9400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="s">
         <v>12</v>
       </c>
@@ -807,8 +954,20 @@
       <c r="E15" s="2">
         <v>2.92E-2</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="5">
+        <v>12.023899999999999</v>
+      </c>
+      <c r="J15" s="1">
+        <v>-1.9446000000000001</v>
+      </c>
+      <c r="K15" s="2">
+        <v>6.2700000000000006E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
         <v>13</v>
       </c>
@@ -821,8 +980,20 @@
       <c r="E16" s="2">
         <v>5.2200000000000003E-2</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="5">
+        <v>11.2227</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1.6848000000000001</v>
+      </c>
+      <c r="K16" s="2">
+        <v>7.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="7" t="s">
         <v>14</v>
       </c>
@@ -835,8 +1006,20 @@
       <c r="E17" s="2">
         <v>1.29E-2</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="5">
+        <v>12.145099999999999</v>
+      </c>
+      <c r="J17" s="1">
+        <v>-3.4935</v>
+      </c>
+      <c r="K17" s="2">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="7" t="s">
         <v>15</v>
       </c>
@@ -849,8 +1032,20 @@
       <c r="E18" s="2">
         <v>1.7100000000000001E-2</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="5">
+        <v>10.3283</v>
+      </c>
+      <c r="J18" s="1">
+        <v>-4.0811000000000002</v>
+      </c>
+      <c r="K18" s="2">
+        <v>9.2700000000000005E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
         <v>16</v>
       </c>
@@ -863,8 +1058,20 @@
       <c r="E19" s="2">
         <v>6.2899999999999998E-2</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="5">
+        <v>10.0288</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1.3008999999999999</v>
+      </c>
+      <c r="K19" s="2">
+        <v>9.9299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>17</v>
       </c>
@@ -877,8 +1084,20 @@
       <c r="E20" s="2">
         <v>2.58E-2</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="5">
+        <v>9.9473000000000003</v>
+      </c>
+      <c r="J20" s="1">
+        <v>-2.6806999999999999</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0.1012</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
         <v>18</v>
       </c>
@@ -891,8 +1110,20 @@
       <c r="E21" s="2">
         <v>2.47E-2</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="5">
+        <v>11.301299999999999</v>
+      </c>
+      <c r="J21" s="1">
+        <v>-1.5024999999999999</v>
+      </c>
+      <c r="K21" s="2">
+        <v>7.4099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>19</v>
       </c>
@@ -904,6 +1135,18 @@
       </c>
       <c r="E22" s="4">
         <v>1.2E-2</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" s="5">
+        <v>12.582000000000001</v>
+      </c>
+      <c r="J22" s="1">
+        <v>-3.4013</v>
+      </c>
+      <c r="K22" s="2">
+        <v>5.5199999999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>